<commit_message>
refined code that deals with JDA detections. re-ran for SY2025 tags
</commit_message>
<xml_diff>
--- a/outgoing/PITcleanr/UC_Steelhead_2025_OKL.xlsx
+++ b/outgoing/PITcleanr/UC_Steelhead_2025_OKL.xlsx
@@ -1214,9 +1214,6 @@
       <c r="O14" t="b">
         <v>0</v>
       </c>
-      <c r="P14" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -36978,9 +36975,6 @@
         </is>
       </c>
       <c r="O611" t="b">
-        <v>0</v>
-      </c>
-      <c r="P611" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>